<commit_message>
Changed "P" to "CFDNA" in the test order form, where appropriate.
</commit_message>
<xml_diff>
--- a/tests/liqbio_test_orderform.xlsx
+++ b/tests/liqbio_test_orderform.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thowhi/repos/autoseq/tests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="211"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="15520" tabRatio="211"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Index" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1763,25 +1771,25 @@
     <t>NA12877-N-03098121-TD1-TT1</t>
   </si>
   <si>
-    <t>NA12877-P-03098850-TD1-TT1</t>
-  </si>
-  <si>
-    <t>NA12877-P-03098850-TD1-TT2</t>
-  </si>
-  <si>
     <t>NA12877-T-03098849-TD1-WGS</t>
   </si>
   <si>
     <t>NA12877-N-03098121-TD1-WGS</t>
   </si>
   <si>
-    <t>NA12877-P-03098850-TD1-WGS</t>
-  </si>
-  <si>
     <t>AL-NA12878-T-sample1-TD1-TT1</t>
   </si>
   <si>
     <t>AL-NA12878-N-sample2-TD1-TT1</t>
+  </si>
+  <si>
+    <t>NA12877-CFDNA-03098850-TD1-TT1</t>
+  </si>
+  <si>
+    <t>NA12877-CFDNA-03098850-TD1-TT2</t>
+  </si>
+  <si>
+    <t>NA12877-CFDNA-03098850-TD1-WGS</t>
   </si>
 </sst>
 </file>
@@ -2893,6 +2901,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3245,7 +3258,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3289,7 +3302,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3314,10 +3327,10 @@
   <dimension ref="A1:XFD46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" hidden="1" customWidth="1"/>
@@ -3337,7 +3350,7 @@
     <col min="20" max="16384" width="13.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16381" ht="22" customHeight="1">
+    <row r="1" spans="1:16381" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
       <c r="C1" s="34"/>
@@ -3360,7 +3373,7 @@
       <c r="R1" s="55"/>
       <c r="S1" s="55"/>
     </row>
-    <row r="2" spans="1:16381" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="2" spans="1:16381" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -3381,7 +3394,7 @@
       <c r="R2" s="56"/>
       <c r="S2" s="56"/>
     </row>
-    <row r="3" spans="1:16381" s="2" customFormat="1" ht="13" customHeight="1">
+    <row r="3" spans="1:16381" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -3403,7 +3416,7 @@
       <c r="R3" s="56"/>
       <c r="S3" s="56"/>
     </row>
-    <row r="4" spans="1:16381" s="2" customFormat="1" ht="17" customHeight="1">
+    <row r="4" spans="1:16381" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="27"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -3424,7 +3437,7 @@
       <c r="R4" s="18"/>
       <c r="S4" s="18"/>
     </row>
-    <row r="5" spans="1:16381">
+    <row r="5" spans="1:16381" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -3435,14 +3448,14 @@
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
     </row>
-    <row r="7" spans="1:16381" ht="16" customHeight="1"/>
-    <row r="8" spans="1:16381" ht="16" hidden="1" customHeight="1"/>
-    <row r="9" spans="1:16381" ht="18" hidden="1" customHeight="1">
+    <row r="7" spans="1:16381" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:16381" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:16381" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16381" s="31" customFormat="1" ht="23" hidden="1" customHeight="1">
+    <row r="10" spans="1:16381" s="31" customFormat="1" ht="23" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
@@ -3501,7 +3514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16381" s="5" customFormat="1" ht="10" hidden="1" customHeight="1">
+    <row r="11" spans="1:16381" s="5" customFormat="1" ht="10" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
         <v>2</v>
       </c>
@@ -3514,7 +3527,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:16381" s="31" customFormat="1" ht="30" customHeight="1">
+    <row r="12" spans="1:16381" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="48" t="s">
         <v>547</v>
       </c>
@@ -19929,7 +19942,7 @@
       <c r="XEZ12" s="29"/>
       <c r="XFA12" s="29"/>
     </row>
-    <row r="13" spans="1:16381" s="5" customFormat="1" ht="13" customHeight="1">
+    <row r="13" spans="1:16381" s="5" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>3</v>
       </c>
@@ -19952,7 +19965,7 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
     </row>
-    <row r="14" spans="1:16381" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="14" spans="1:16381" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="53" t="s">
         <v>578</v>
       </c>
@@ -20014,7 +20027,7 @@
       <c r="AG14" s="46"/>
       <c r="AH14" s="46"/>
     </row>
-    <row r="15" spans="1:16381" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="15" spans="1:16381" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="53" t="s">
         <v>579</v>
       </c>
@@ -20076,9 +20089,9 @@
       <c r="AG15" s="46"/>
       <c r="AH15" s="46"/>
     </row>
-    <row r="16" spans="1:16381" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="16" spans="1:16381" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="53" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="B16" s="42" t="s">
         <v>33</v>
@@ -20138,9 +20151,9 @@
       <c r="AG16" s="46"/>
       <c r="AH16" s="46"/>
     </row>
-    <row r="17" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="17" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="53" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="B17" s="42" t="s">
         <v>33</v>
@@ -20200,9 +20213,9 @@
       <c r="AG17" s="46"/>
       <c r="AH17" s="46"/>
     </row>
-    <row r="18" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="18" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="53" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>33</v>
@@ -20262,9 +20275,9 @@
       <c r="AG18" s="46"/>
       <c r="AH18" s="46"/>
     </row>
-    <row r="19" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="19" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="53" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>33</v>
@@ -20324,9 +20337,9 @@
       <c r="AG19" s="46"/>
       <c r="AH19" s="46"/>
     </row>
-    <row r="20" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1">
+    <row r="20" spans="1:16384" s="47" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="53" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>33</v>
@@ -20386,9 +20399,9 @@
       <c r="AG20" s="46"/>
       <c r="AH20" s="46"/>
     </row>
-    <row r="21" spans="1:16384" s="46" customFormat="1" ht="13" customHeight="1">
+    <row r="21" spans="1:16384" s="46" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="53" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B21" s="54"/>
       <c r="C21" s="42" t="s">
@@ -36781,9 +36794,9 @@
       <c r="XFC21" s="47"/>
       <c r="XFD21" s="47"/>
     </row>
-    <row r="22" spans="1:16384" s="46" customFormat="1" ht="13" customHeight="1">
+    <row r="22" spans="1:16384" s="46" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="53" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B22" s="54"/>
       <c r="C22" s="42" t="s">
@@ -53176,17 +53189,17 @@
       <c r="XFC22" s="47"/>
       <c r="XFD22" s="47"/>
     </row>
-    <row r="23" spans="1:16384">
+    <row r="23" spans="1:16384" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:16384">
+    <row r="24" spans="1:16384" x14ac:dyDescent="0.15">
       <c r="A24" s="8"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:16384" s="14" customFormat="1" ht="12">
+    <row r="25" spans="1:16384" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
         <v>11</v>
       </c>
@@ -53209,7 +53222,7 @@
       <c r="R25" s="16"/>
       <c r="S25" s="16"/>
     </row>
-    <row r="26" spans="1:16384" s="14" customFormat="1" ht="12">
+    <row r="26" spans="1:16384" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
         <v>12</v>
       </c>
@@ -53232,7 +53245,7 @@
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
     </row>
-    <row r="27" spans="1:16384" s="14" customFormat="1" ht="12">
+    <row r="27" spans="1:16384" s="14" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="13" t="s">
         <v>20</v>
       </c>
@@ -53255,13 +53268,13 @@
       <c r="R27" s="16"/>
       <c r="S27" s="16"/>
     </row>
-    <row r="28" spans="1:16384">
+    <row r="28" spans="1:16384" x14ac:dyDescent="0.15">
       <c r="E28" s="17"/>
     </row>
-    <row r="29" spans="1:16384">
+    <row r="29" spans="1:16384" x14ac:dyDescent="0.15">
       <c r="E29" s="17"/>
     </row>
-    <row r="30" spans="1:16384" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="30" spans="1:16384" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -53282,7 +53295,7 @@
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
     </row>
-    <row r="31" spans="1:16384" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="31" spans="1:16384" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -53303,7 +53316,7 @@
       <c r="R31" s="17"/>
       <c r="S31" s="17"/>
     </row>
-    <row r="32" spans="1:16384" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="32" spans="1:16384" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -53324,7 +53337,7 @@
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="33" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -53345,7 +53358,7 @@
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
     </row>
-    <row r="34" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="34" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -53366,7 +53379,7 @@
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
     </row>
-    <row r="35" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="35" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -53386,7 +53399,7 @@
       <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
     </row>
-    <row r="36" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="36" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
@@ -53406,7 +53419,7 @@
       <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
     </row>
-    <row r="37" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="37" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
@@ -53426,7 +53439,7 @@
       <c r="Q37" s="17"/>
       <c r="R37" s="17"/>
     </row>
-    <row r="38" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="38" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -53446,7 +53459,7 @@
       <c r="Q38" s="17"/>
       <c r="R38" s="17"/>
     </row>
-    <row r="39" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="39" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -53466,7 +53479,7 @@
       <c r="Q39" s="17"/>
       <c r="R39" s="17"/>
     </row>
-    <row r="40" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1">
+    <row r="40" spans="1:19" s="16" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -53486,7 +53499,7 @@
       <c r="Q40" s="17"/>
       <c r="R40" s="17"/>
     </row>
-    <row r="41" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1">
+    <row r="41" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -53506,7 +53519,7 @@
       <c r="Q41" s="17"/>
       <c r="R41" s="17"/>
     </row>
-    <row r="42" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1">
+    <row r="42" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -53526,7 +53539,7 @@
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
     </row>
-    <row r="43" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1">
+    <row r="43" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -53546,7 +53559,7 @@
       <c r="Q43" s="17"/>
       <c r="R43" s="17"/>
     </row>
-    <row r="44" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1">
+    <row r="44" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -53566,7 +53579,7 @@
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
     </row>
-    <row r="45" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1">
+    <row r="45" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -53586,7 +53599,7 @@
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
     </row>
-    <row r="46" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1">
+    <row r="46" spans="1:19" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -53663,9 +53676,6 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -53678,7 +53688,7 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="36.5" customWidth="1"/>
     <col min="7" max="7" width="22.1640625" customWidth="1"/>
@@ -53690,7 +53700,7 @@
     <col min="13" max="13" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -53713,7 +53723,7 @@
       <c r="L1" s="35"/>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -53736,7 +53746,7 @@
       <c r="L2" s="37"/>
       <c r="M2" s="37"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>16</v>
       </c>
@@ -53753,7 +53763,7 @@
       <c r="L3" s="40"/>
       <c r="M3" s="40"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D4" s="32" t="s">
         <v>27</v>
       </c>
@@ -53767,7 +53777,7 @@
       <c r="L4" s="40"/>
       <c r="M4" s="40"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D5" s="32" t="s">
         <v>28</v>
       </c>
@@ -53781,7 +53791,7 @@
       <c r="L5" s="40"/>
       <c r="M5" s="40"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D6" s="32" t="s">
         <v>29</v>
       </c>
@@ -53795,7 +53805,7 @@
       <c r="L6" s="40"/>
       <c r="M6" s="40"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D7" s="32" t="s">
         <v>30</v>
       </c>
@@ -53809,7 +53819,7 @@
       <c r="L7" s="40"/>
       <c r="M7" s="40"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D8" s="32" t="s">
         <v>31</v>
       </c>
@@ -53823,7 +53833,7 @@
       <c r="L8" s="40"/>
       <c r="M8" s="40"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E9" s="38"/>
       <c r="F9" s="39"/>
       <c r="G9" s="40"/>
@@ -53834,7 +53844,7 @@
       <c r="L9" s="40"/>
       <c r="M9" s="40"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E10" s="38"/>
       <c r="F10" s="39"/>
       <c r="G10" s="40"/>
@@ -53845,7 +53855,7 @@
       <c r="L10" s="40"/>
       <c r="M10" s="40"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E11" s="38"/>
       <c r="F11" s="39"/>
       <c r="G11" s="40"/>
@@ -53856,7 +53866,7 @@
       <c r="L11" s="40"/>
       <c r="M11" s="40"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E12" s="38"/>
       <c r="F12" s="39"/>
       <c r="G12" s="40"/>
@@ -53867,7 +53877,7 @@
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D13" t="s">
         <v>15</v>
       </c>
@@ -53881,7 +53891,7 @@
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>568</v>
       </c>
@@ -53898,7 +53908,7 @@
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>570</v>
       </c>
@@ -53915,7 +53925,7 @@
       <c r="L15" s="40"/>
       <c r="M15" s="40"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>569</v>
       </c>
@@ -53929,7 +53939,7 @@
       <c r="L16" s="40"/>
       <c r="M16" s="40"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>573</v>
       </c>
@@ -53943,7 +53953,7 @@
       <c r="L17" s="40"/>
       <c r="M17" s="40"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>574</v>
       </c>
@@ -53957,7 +53967,7 @@
       <c r="L18" s="40"/>
       <c r="M18" s="40"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>575</v>
       </c>
@@ -53971,7 +53981,7 @@
       <c r="L19" s="40"/>
       <c r="M19" s="40"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>571</v>
       </c>
@@ -53985,7 +53995,7 @@
       <c r="L20" s="40"/>
       <c r="M20" s="40"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E21" s="38"/>
       <c r="F21" s="39"/>
       <c r="G21" s="40"/>
@@ -53996,7 +54006,7 @@
       <c r="L21" s="40"/>
       <c r="M21" s="40"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D22" t="s">
         <v>538</v>
       </c>
@@ -54010,7 +54020,7 @@
       <c r="L22" s="40"/>
       <c r="M22" s="38"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D23" t="s">
         <v>539</v>
       </c>
@@ -54024,7 +54034,7 @@
       <c r="L23" s="40"/>
       <c r="M23" s="38"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D24" t="s">
         <v>540</v>
       </c>
@@ -54038,7 +54048,7 @@
       <c r="L24" s="40"/>
       <c r="M24" s="38"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D25" t="s">
         <v>544</v>
       </c>
@@ -54054,7 +54064,7 @@
       <c r="L25" s="40"/>
       <c r="M25" s="38"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E26" s="38">
         <v>2</v>
       </c>
@@ -54067,7 +54077,7 @@
       <c r="L26" s="40"/>
       <c r="M26" s="38"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E27" s="38">
         <v>3</v>
       </c>
@@ -54080,7 +54090,7 @@
       <c r="L27" s="40"/>
       <c r="M27" s="38"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E28" s="38">
         <v>4</v>
       </c>
@@ -54093,7 +54103,7 @@
       <c r="L28" s="40"/>
       <c r="M28" s="38"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D29" t="s">
         <v>542</v>
       </c>
@@ -54109,7 +54119,7 @@
       <c r="L29" s="40"/>
       <c r="M29" s="38"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="D30" t="s">
         <v>543</v>
       </c>
@@ -54125,7 +54135,7 @@
       <c r="L30" s="40"/>
       <c r="M30" s="38"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E31" s="38">
         <v>7</v>
       </c>
@@ -54138,7 +54148,7 @@
       <c r="L31" s="40"/>
       <c r="M31" s="38"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E32" s="38">
         <v>8</v>
       </c>
@@ -54151,7 +54161,7 @@
       <c r="L32" s="40"/>
       <c r="M32" s="38"/>
     </row>
-    <row r="33" spans="5:13">
+    <row r="33" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E33" s="38">
         <v>9</v>
       </c>
@@ -54164,7 +54174,7 @@
       <c r="L33" s="40"/>
       <c r="M33" s="38"/>
     </row>
-    <row r="34" spans="5:13">
+    <row r="34" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E34" s="38">
         <v>10</v>
       </c>
@@ -54177,7 +54187,7 @@
       <c r="L34" s="40"/>
       <c r="M34" s="38"/>
     </row>
-    <row r="35" spans="5:13">
+    <row r="35" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E35" s="38"/>
       <c r="F35" s="39"/>
       <c r="G35" s="40"/>
@@ -54188,7 +54198,7 @@
       <c r="L35" s="40"/>
       <c r="M35" s="38"/>
     </row>
-    <row r="36" spans="5:13">
+    <row r="36" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E36" s="38"/>
       <c r="F36" s="39"/>
       <c r="G36" s="40"/>
@@ -54199,7 +54209,7 @@
       <c r="L36" s="40"/>
       <c r="M36" s="38"/>
     </row>
-    <row r="37" spans="5:13">
+    <row r="37" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E37" s="38"/>
       <c r="F37" s="39"/>
       <c r="G37" s="40"/>
@@ -54210,7 +54220,7 @@
       <c r="L37" s="40"/>
       <c r="M37" s="38"/>
     </row>
-    <row r="38" spans="5:13">
+    <row r="38" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E38" s="38"/>
       <c r="F38" s="39"/>
       <c r="G38" s="40"/>
@@ -54221,7 +54231,7 @@
       <c r="L38" s="40"/>
       <c r="M38" s="38"/>
     </row>
-    <row r="39" spans="5:13">
+    <row r="39" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E39" s="38"/>
       <c r="F39" s="39"/>
       <c r="G39" s="40"/>
@@ -54232,7 +54242,7 @@
       <c r="L39" s="40"/>
       <c r="M39" s="38"/>
     </row>
-    <row r="40" spans="5:13">
+    <row r="40" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E40" s="38"/>
       <c r="F40" s="39"/>
       <c r="G40" s="40"/>
@@ -54243,7 +54253,7 @@
       <c r="L40" s="40"/>
       <c r="M40" s="38"/>
     </row>
-    <row r="41" spans="5:13">
+    <row r="41" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E41" s="38"/>
       <c r="F41" s="39"/>
       <c r="G41" s="40"/>
@@ -54254,7 +54264,7 @@
       <c r="L41" s="40"/>
       <c r="M41" s="38"/>
     </row>
-    <row r="42" spans="5:13">
+    <row r="42" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E42" s="38"/>
       <c r="F42" s="39"/>
       <c r="G42" s="40"/>
@@ -54265,7 +54275,7 @@
       <c r="L42" s="40"/>
       <c r="M42" s="38"/>
     </row>
-    <row r="43" spans="5:13">
+    <row r="43" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E43" s="38"/>
       <c r="F43" s="39"/>
       <c r="G43" s="40"/>
@@ -54276,7 +54286,7 @@
       <c r="L43" s="40"/>
       <c r="M43" s="38"/>
     </row>
-    <row r="44" spans="5:13">
+    <row r="44" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E44" s="38"/>
       <c r="F44" s="39"/>
       <c r="G44" s="40"/>
@@ -54287,7 +54297,7 @@
       <c r="L44" s="40"/>
       <c r="M44" s="38"/>
     </row>
-    <row r="45" spans="5:13">
+    <row r="45" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E45" s="38"/>
       <c r="F45" s="39"/>
       <c r="G45" s="40"/>
@@ -54298,7 +54308,7 @@
       <c r="L45" s="40"/>
       <c r="M45" s="38"/>
     </row>
-    <row r="46" spans="5:13">
+    <row r="46" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E46" s="38"/>
       <c r="F46" s="39"/>
       <c r="G46" s="40"/>
@@ -54309,7 +54319,7 @@
       <c r="L46" s="40"/>
       <c r="M46" s="38"/>
     </row>
-    <row r="47" spans="5:13">
+    <row r="47" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E47" s="38"/>
       <c r="F47" s="39"/>
       <c r="G47" s="40"/>
@@ -54320,7 +54330,7 @@
       <c r="L47" s="40"/>
       <c r="M47" s="38"/>
     </row>
-    <row r="48" spans="5:13">
+    <row r="48" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E48" s="38"/>
       <c r="F48" s="39"/>
       <c r="G48" s="40"/>
@@ -54331,7 +54341,7 @@
       <c r="L48" s="40"/>
       <c r="M48" s="38"/>
     </row>
-    <row r="49" spans="5:13">
+    <row r="49" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E49" s="38"/>
       <c r="F49" s="39"/>
       <c r="G49" s="40"/>
@@ -54342,7 +54352,7 @@
       <c r="L49" s="40"/>
       <c r="M49" s="38"/>
     </row>
-    <row r="50" spans="5:13">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E50" s="38"/>
       <c r="F50" s="39"/>
       <c r="G50" s="40"/>
@@ -54353,7 +54363,7 @@
       <c r="L50" s="40"/>
       <c r="M50" s="38"/>
     </row>
-    <row r="51" spans="5:13">
+    <row r="51" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E51" s="38"/>
       <c r="F51" s="39"/>
       <c r="G51" s="40"/>
@@ -54364,7 +54374,7 @@
       <c r="L51" s="40"/>
       <c r="M51" s="38"/>
     </row>
-    <row r="52" spans="5:13">
+    <row r="52" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E52" s="38"/>
       <c r="F52" s="39"/>
       <c r="G52" s="40"/>
@@ -54375,7 +54385,7 @@
       <c r="L52" s="40"/>
       <c r="M52" s="38"/>
     </row>
-    <row r="53" spans="5:13">
+    <row r="53" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E53" s="38"/>
       <c r="F53" s="39"/>
       <c r="G53" s="40"/>
@@ -54386,7 +54396,7 @@
       <c r="L53" s="40"/>
       <c r="M53" s="38"/>
     </row>
-    <row r="54" spans="5:13">
+    <row r="54" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E54" s="38"/>
       <c r="F54" s="39"/>
       <c r="G54" s="40"/>
@@ -54397,7 +54407,7 @@
       <c r="L54" s="38"/>
       <c r="M54" s="38"/>
     </row>
-    <row r="55" spans="5:13">
+    <row r="55" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E55" s="38"/>
       <c r="F55" s="39"/>
       <c r="G55" s="40"/>
@@ -54408,7 +54418,7 @@
       <c r="L55" s="38"/>
       <c r="M55" s="38"/>
     </row>
-    <row r="56" spans="5:13">
+    <row r="56" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E56" s="38"/>
       <c r="F56" s="39"/>
       <c r="G56" s="40"/>
@@ -54419,7 +54429,7 @@
       <c r="L56" s="38"/>
       <c r="M56" s="38"/>
     </row>
-    <row r="57" spans="5:13">
+    <row r="57" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E57" s="38"/>
       <c r="F57" s="39"/>
       <c r="G57" s="40"/>
@@ -54430,7 +54440,7 @@
       <c r="L57" s="38"/>
       <c r="M57" s="38"/>
     </row>
-    <row r="58" spans="5:13">
+    <row r="58" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E58" s="38"/>
       <c r="F58" s="39"/>
       <c r="G58" s="40"/>
@@ -54441,7 +54451,7 @@
       <c r="L58" s="38"/>
       <c r="M58" s="38"/>
     </row>
-    <row r="59" spans="5:13">
+    <row r="59" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E59" s="38"/>
       <c r="F59" s="39"/>
       <c r="G59" s="40"/>
@@ -54452,7 +54462,7 @@
       <c r="L59" s="38"/>
       <c r="M59" s="38"/>
     </row>
-    <row r="60" spans="5:13">
+    <row r="60" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E60" s="38"/>
       <c r="F60" s="39"/>
       <c r="G60" s="40"/>
@@ -54463,7 +54473,7 @@
       <c r="L60" s="38"/>
       <c r="M60" s="38"/>
     </row>
-    <row r="61" spans="5:13">
+    <row r="61" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E61" s="38"/>
       <c r="F61" s="39"/>
       <c r="G61" s="40"/>
@@ -54474,7 +54484,7 @@
       <c r="L61" s="38"/>
       <c r="M61" s="38"/>
     </row>
-    <row r="62" spans="5:13">
+    <row r="62" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E62" s="38"/>
       <c r="F62" s="39"/>
       <c r="G62" s="40"/>
@@ -54485,7 +54495,7 @@
       <c r="L62" s="38"/>
       <c r="M62" s="38"/>
     </row>
-    <row r="63" spans="5:13">
+    <row r="63" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E63" s="38"/>
       <c r="F63" s="39"/>
       <c r="G63" s="40"/>
@@ -54496,7 +54506,7 @@
       <c r="L63" s="38"/>
       <c r="M63" s="38"/>
     </row>
-    <row r="64" spans="5:13">
+    <row r="64" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E64" s="38"/>
       <c r="F64" s="39"/>
       <c r="G64" s="40"/>
@@ -54507,7 +54517,7 @@
       <c r="L64" s="38"/>
       <c r="M64" s="38"/>
     </row>
-    <row r="65" spans="5:13">
+    <row r="65" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E65" s="38"/>
       <c r="F65" s="39"/>
       <c r="G65" s="40"/>
@@ -54518,7 +54528,7 @@
       <c r="L65" s="38"/>
       <c r="M65" s="38"/>
     </row>
-    <row r="66" spans="5:13">
+    <row r="66" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E66" s="38"/>
       <c r="F66" s="39"/>
       <c r="G66" s="40"/>
@@ -54529,7 +54539,7 @@
       <c r="L66" s="38"/>
       <c r="M66" s="38"/>
     </row>
-    <row r="67" spans="5:13">
+    <row r="67" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E67" s="38"/>
       <c r="F67" s="39"/>
       <c r="G67" s="40"/>
@@ -54540,7 +54550,7 @@
       <c r="L67" s="38"/>
       <c r="M67" s="38"/>
     </row>
-    <row r="68" spans="5:13">
+    <row r="68" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E68" s="38"/>
       <c r="F68" s="39"/>
       <c r="G68" s="40"/>
@@ -54551,7 +54561,7 @@
       <c r="L68" s="38"/>
       <c r="M68" s="38"/>
     </row>
-    <row r="69" spans="5:13">
+    <row r="69" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E69" s="38"/>
       <c r="F69" s="39"/>
       <c r="G69" s="40"/>
@@ -54562,7 +54572,7 @@
       <c r="L69" s="38"/>
       <c r="M69" s="38"/>
     </row>
-    <row r="70" spans="5:13">
+    <row r="70" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E70" s="38"/>
       <c r="F70" s="39"/>
       <c r="G70" s="40"/>
@@ -54573,7 +54583,7 @@
       <c r="L70" s="38"/>
       <c r="M70" s="38"/>
     </row>
-    <row r="71" spans="5:13">
+    <row r="71" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E71" s="38"/>
       <c r="F71" s="39"/>
       <c r="G71" s="40"/>
@@ -54584,7 +54594,7 @@
       <c r="L71" s="38"/>
       <c r="M71" s="38"/>
     </row>
-    <row r="72" spans="5:13">
+    <row r="72" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E72" s="38"/>
       <c r="F72" s="39"/>
       <c r="G72" s="40"/>
@@ -54595,7 +54605,7 @@
       <c r="L72" s="38"/>
       <c r="M72" s="38"/>
     </row>
-    <row r="73" spans="5:13">
+    <row r="73" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E73" s="38"/>
       <c r="F73" s="39"/>
       <c r="G73" s="40"/>
@@ -54606,7 +54616,7 @@
       <c r="L73" s="38"/>
       <c r="M73" s="38"/>
     </row>
-    <row r="74" spans="5:13">
+    <row r="74" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E74" s="38"/>
       <c r="F74" s="39"/>
       <c r="G74" s="40"/>
@@ -54617,7 +54627,7 @@
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
     </row>
-    <row r="75" spans="5:13">
+    <row r="75" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E75" s="38"/>
       <c r="F75" s="39"/>
       <c r="G75" s="40"/>
@@ -54628,7 +54638,7 @@
       <c r="L75" s="38"/>
       <c r="M75" s="38"/>
     </row>
-    <row r="76" spans="5:13">
+    <row r="76" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E76" s="38"/>
       <c r="F76" s="39"/>
       <c r="G76" s="40"/>
@@ -54639,7 +54649,7 @@
       <c r="L76" s="38"/>
       <c r="M76" s="38"/>
     </row>
-    <row r="77" spans="5:13">
+    <row r="77" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E77" s="38"/>
       <c r="F77" s="39"/>
       <c r="G77" s="40"/>
@@ -54650,7 +54660,7 @@
       <c r="L77" s="38"/>
       <c r="M77" s="38"/>
     </row>
-    <row r="78" spans="5:13">
+    <row r="78" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E78" s="38"/>
       <c r="F78" s="39"/>
       <c r="G78" s="40"/>
@@ -54661,7 +54671,7 @@
       <c r="L78" s="38"/>
       <c r="M78" s="38"/>
     </row>
-    <row r="79" spans="5:13">
+    <row r="79" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E79" s="38"/>
       <c r="F79" s="39"/>
       <c r="G79" s="40"/>
@@ -54672,7 +54682,7 @@
       <c r="L79" s="38"/>
       <c r="M79" s="38"/>
     </row>
-    <row r="80" spans="5:13">
+    <row r="80" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E80" s="38"/>
       <c r="F80" s="39"/>
       <c r="G80" s="40"/>
@@ -54683,7 +54693,7 @@
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
     </row>
-    <row r="81" spans="5:13">
+    <row r="81" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E81" s="38"/>
       <c r="F81" s="39"/>
       <c r="G81" s="40"/>
@@ -54694,7 +54704,7 @@
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
     </row>
-    <row r="82" spans="5:13">
+    <row r="82" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E82" s="38"/>
       <c r="F82" s="39"/>
       <c r="G82" s="40"/>
@@ -54705,7 +54715,7 @@
       <c r="L82" s="38"/>
       <c r="M82" s="38"/>
     </row>
-    <row r="83" spans="5:13">
+    <row r="83" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E83" s="38"/>
       <c r="F83" s="39"/>
       <c r="G83" s="40"/>
@@ -54716,7 +54726,7 @@
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>
     </row>
-    <row r="84" spans="5:13">
+    <row r="84" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E84" s="38"/>
       <c r="F84" s="39"/>
       <c r="G84" s="40"/>
@@ -54727,7 +54737,7 @@
       <c r="L84" s="38"/>
       <c r="M84" s="38"/>
     </row>
-    <row r="85" spans="5:13">
+    <row r="85" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E85" s="38"/>
       <c r="F85" s="39"/>
       <c r="G85" s="40"/>
@@ -54738,7 +54748,7 @@
       <c r="L85" s="38"/>
       <c r="M85" s="38"/>
     </row>
-    <row r="86" spans="5:13">
+    <row r="86" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E86" s="38"/>
       <c r="F86" s="39"/>
       <c r="G86" s="40"/>
@@ -54749,7 +54759,7 @@
       <c r="L86" s="38"/>
       <c r="M86" s="38"/>
     </row>
-    <row r="87" spans="5:13">
+    <row r="87" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E87" s="38"/>
       <c r="F87" s="39"/>
       <c r="G87" s="40"/>
@@ -54760,7 +54770,7 @@
       <c r="L87" s="38"/>
       <c r="M87" s="38"/>
     </row>
-    <row r="88" spans="5:13">
+    <row r="88" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E88" s="38"/>
       <c r="F88" s="39"/>
       <c r="G88" s="40"/>
@@ -54771,7 +54781,7 @@
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
     </row>
-    <row r="89" spans="5:13">
+    <row r="89" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E89" s="38"/>
       <c r="F89" s="39"/>
       <c r="G89" s="40"/>
@@ -54782,7 +54792,7 @@
       <c r="L89" s="38"/>
       <c r="M89" s="38"/>
     </row>
-    <row r="90" spans="5:13">
+    <row r="90" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E90" s="38"/>
       <c r="F90" s="39"/>
       <c r="G90" s="40"/>
@@ -54793,7 +54803,7 @@
       <c r="L90" s="38"/>
       <c r="M90" s="38"/>
     </row>
-    <row r="91" spans="5:13">
+    <row r="91" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E91" s="38"/>
       <c r="F91" s="39"/>
       <c r="G91" s="40"/>
@@ -54804,7 +54814,7 @@
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
     </row>
-    <row r="92" spans="5:13">
+    <row r="92" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E92" s="38"/>
       <c r="F92" s="39"/>
       <c r="G92" s="40"/>
@@ -54815,7 +54825,7 @@
       <c r="L92" s="38"/>
       <c r="M92" s="38"/>
     </row>
-    <row r="93" spans="5:13">
+    <row r="93" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E93" s="38"/>
       <c r="F93" s="39"/>
       <c r="G93" s="40"/>
@@ -54826,7 +54836,7 @@
       <c r="L93" s="38"/>
       <c r="M93" s="38"/>
     </row>
-    <row r="94" spans="5:13">
+    <row r="94" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E94" s="38"/>
       <c r="F94" s="39"/>
       <c r="G94" s="40"/>
@@ -54837,7 +54847,7 @@
       <c r="L94" s="38"/>
       <c r="M94" s="38"/>
     </row>
-    <row r="95" spans="5:13">
+    <row r="95" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E95" s="38"/>
       <c r="F95" s="39"/>
       <c r="G95" s="40"/>
@@ -54848,7 +54858,7 @@
       <c r="L95" s="38"/>
       <c r="M95" s="38"/>
     </row>
-    <row r="96" spans="5:13">
+    <row r="96" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E96" s="38"/>
       <c r="F96" s="39"/>
       <c r="G96" s="40"/>
@@ -54859,7 +54869,7 @@
       <c r="L96" s="38"/>
       <c r="M96" s="38"/>
     </row>
-    <row r="97" spans="5:13">
+    <row r="97" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E97" s="38"/>
       <c r="F97" s="39"/>
       <c r="G97" s="40"/>
@@ -54870,7 +54880,7 @@
       <c r="L97" s="38"/>
       <c r="M97" s="38"/>
     </row>
-    <row r="98" spans="5:13">
+    <row r="98" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E98" s="38"/>
       <c r="F98" s="39"/>
       <c r="G98" s="40"/>
@@ -54881,7 +54891,7 @@
       <c r="L98" s="38"/>
       <c r="M98" s="38"/>
     </row>
-    <row r="99" spans="5:13">
+    <row r="99" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E99" s="38"/>
       <c r="F99" s="39"/>
       <c r="G99" s="40"/>
@@ -54892,7 +54902,7 @@
       <c r="L99" s="38"/>
       <c r="M99" s="38"/>
     </row>
-    <row r="100" spans="5:13">
+    <row r="100" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E100" s="38"/>
       <c r="F100" s="39"/>
       <c r="G100" s="40"/>
@@ -54903,7 +54913,7 @@
       <c r="L100" s="38"/>
       <c r="M100" s="38"/>
     </row>
-    <row r="101" spans="5:13">
+    <row r="101" spans="5:13" x14ac:dyDescent="0.15">
       <c r="E101" s="38"/>
       <c r="F101" s="39"/>
       <c r="G101" s="40"/>
@@ -54917,11 +54927,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -54933,7 +54938,7 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="35" style="41" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="41" customWidth="1"/>
@@ -54947,7 +54952,7 @@
     <col min="10" max="16384" width="17.1640625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -54962,7 +54967,7 @@
       <c r="H1" s="35"/>
       <c r="I1" s="35"/>
     </row>
-    <row r="2" spans="1:9" ht="12" customHeight="1">
+    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="36" t="s">
         <v>37</v>
       </c>
@@ -54991,7 +54996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12">
+    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>25</v>
       </c>
@@ -55020,7 +55025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12">
+    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="38" t="s">
         <v>24</v>
       </c>
@@ -55049,7 +55054,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12">
+    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="38" t="s">
         <v>39</v>
       </c>
@@ -55078,7 +55083,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12">
+    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="38" t="s">
         <v>26</v>
       </c>
@@ -55107,7 +55112,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12">
+    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="38" t="s">
         <v>27</v>
       </c>
@@ -55136,7 +55141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12">
+    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
         <v>28</v>
       </c>
@@ -55165,7 +55170,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12">
+    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="38" t="s">
         <v>29</v>
       </c>
@@ -55194,7 +55199,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12">
+    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="38" t="s">
         <v>30</v>
       </c>
@@ -55223,7 +55228,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12">
+    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="38" t="s">
         <v>31</v>
       </c>
@@ -55252,7 +55257,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12">
+    <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="38"/>
       <c r="B12" s="39">
         <v>10</v>
@@ -55279,7 +55284,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12">
+    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="38"/>
       <c r="B13" s="39">
         <v>11</v>
@@ -55306,7 +55311,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12">
+    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="38"/>
       <c r="B14" s="39">
         <v>12</v>
@@ -55333,7 +55338,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12">
+    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="38"/>
       <c r="B15" s="39">
         <v>13</v>
@@ -55360,7 +55365,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12">
+    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="38"/>
       <c r="B16" s="39">
         <v>14</v>
@@ -55387,7 +55392,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12">
+    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="38"/>
       <c r="B17" s="39">
         <v>15</v>
@@ -55414,7 +55419,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="12">
+    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="38"/>
       <c r="B18" s="39">
         <v>16</v>
@@ -55441,7 +55446,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="12">
+    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="38"/>
       <c r="B19" s="39">
         <v>17</v>
@@ -55468,7 +55473,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="12">
+    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="38"/>
       <c r="B20" s="39">
         <v>18</v>
@@ -55495,7 +55500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="12">
+    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="38"/>
       <c r="B21" s="39">
         <v>19</v>
@@ -55522,7 +55527,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="12">
+    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="38"/>
       <c r="B22" s="39">
         <v>20</v>
@@ -55549,7 +55554,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="12">
+    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="38"/>
       <c r="B23" s="39">
         <v>21</v>
@@ -55576,7 +55581,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="12">
+    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="38"/>
       <c r="B24" s="39">
         <v>22</v>
@@ -55603,7 +55608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="12">
+    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="38"/>
       <c r="B25" s="39">
         <v>23</v>
@@ -55630,7 +55635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="12">
+    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="38"/>
       <c r="B26" s="39">
         <v>24</v>
@@ -55657,7 +55662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="12">
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="38"/>
       <c r="B27" s="39">
         <v>25</v>
@@ -55684,7 +55689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="12">
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="38"/>
       <c r="B28" s="39">
         <v>26</v>
@@ -55711,7 +55716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="12">
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="38"/>
       <c r="B29" s="39">
         <v>27</v>
@@ -55738,7 +55743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="12">
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="38"/>
       <c r="B30" s="39">
         <v>28</v>
@@ -55765,7 +55770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="12">
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="38"/>
       <c r="B31" s="39">
         <v>29</v>
@@ -55792,7 +55797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="12">
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="38"/>
       <c r="B32" s="39">
         <v>30</v>
@@ -55819,7 +55824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="12">
+    <row r="33" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="38"/>
       <c r="B33" s="39">
         <v>31</v>
@@ -55846,7 +55851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="12">
+    <row r="34" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="38"/>
       <c r="B34" s="39">
         <v>32</v>
@@ -55873,7 +55878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="12">
+    <row r="35" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="38"/>
       <c r="B35" s="39">
         <v>33</v>
@@ -55900,7 +55905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="12">
+    <row r="36" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="38"/>
       <c r="B36" s="39">
         <v>34</v>
@@ -55927,7 +55932,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="12">
+    <row r="37" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="38"/>
       <c r="B37" s="39">
         <v>35</v>
@@ -55954,7 +55959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="12">
+    <row r="38" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="38"/>
       <c r="B38" s="39">
         <v>36</v>
@@ -55981,7 +55986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="12">
+    <row r="39" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="38"/>
       <c r="B39" s="39">
         <v>37</v>
@@ -56008,7 +56013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="12">
+    <row r="40" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="38"/>
       <c r="B40" s="39">
         <v>38</v>
@@ -56035,7 +56040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="12">
+    <row r="41" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="38"/>
       <c r="B41" s="39">
         <v>39</v>
@@ -56062,7 +56067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="12">
+    <row r="42" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="38"/>
       <c r="B42" s="39">
         <v>40</v>
@@ -56089,7 +56094,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="12">
+    <row r="43" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="38"/>
       <c r="B43" s="39">
         <v>41</v>
@@ -56116,7 +56121,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="12">
+    <row r="44" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="38"/>
       <c r="B44" s="39">
         <v>42</v>
@@ -56143,7 +56148,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="12">
+    <row r="45" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="38"/>
       <c r="B45" s="39">
         <v>43</v>
@@ -56170,7 +56175,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="12">
+    <row r="46" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="38"/>
       <c r="B46" s="39">
         <v>44</v>
@@ -56197,7 +56202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="12">
+    <row r="47" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="38"/>
       <c r="B47" s="39">
         <v>45</v>
@@ -56224,7 +56229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="12">
+    <row r="48" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="38"/>
       <c r="B48" s="39">
         <v>46</v>
@@ -56251,7 +56256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="12">
+    <row r="49" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="38"/>
       <c r="B49" s="39">
         <v>47</v>
@@ -56278,7 +56283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="12">
+    <row r="50" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="38"/>
       <c r="B50" s="39">
         <v>48</v>
@@ -56305,7 +56310,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="12">
+    <row r="51" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="38"/>
       <c r="B51" s="39">
         <v>49</v>
@@ -56332,7 +56337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="12">
+    <row r="52" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="38"/>
       <c r="B52" s="39">
         <v>50</v>
@@ -56359,7 +56364,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="12">
+    <row r="53" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="38"/>
       <c r="B53" s="39">
         <v>51</v>
@@ -56386,7 +56391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="12">
+    <row r="54" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="38"/>
       <c r="B54" s="39">
         <v>52</v>
@@ -56413,7 +56418,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="12">
+    <row r="55" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="38"/>
       <c r="B55" s="39">
         <v>53</v>
@@ -56440,7 +56445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="12">
+    <row r="56" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="38"/>
       <c r="B56" s="39">
         <v>54</v>
@@ -56467,7 +56472,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="12">
+    <row r="57" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="38"/>
       <c r="B57" s="39">
         <v>55</v>
@@ -56494,7 +56499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="12">
+    <row r="58" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="38"/>
       <c r="B58" s="39">
         <v>56</v>
@@ -56521,7 +56526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="12">
+    <row r="59" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="38"/>
       <c r="B59" s="39">
         <v>57</v>
@@ -56548,7 +56553,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="12">
+    <row r="60" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="38"/>
       <c r="B60" s="39">
         <v>58</v>
@@ -56575,7 +56580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="12">
+    <row r="61" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="38"/>
       <c r="B61" s="39">
         <v>59</v>
@@ -56602,7 +56607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="12">
+    <row r="62" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="38"/>
       <c r="B62" s="39">
         <v>60</v>
@@ -56629,7 +56634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="12">
+    <row r="63" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="38"/>
       <c r="B63" s="39">
         <v>61</v>
@@ -56656,7 +56661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="12">
+    <row r="64" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="38"/>
       <c r="B64" s="39">
         <v>62</v>
@@ -56683,7 +56688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="12">
+    <row r="65" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="38"/>
       <c r="B65" s="39">
         <v>63</v>
@@ -56710,7 +56715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="12">
+    <row r="66" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="38"/>
       <c r="B66" s="39">
         <v>64</v>
@@ -56737,7 +56742,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="12">
+    <row r="67" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="38"/>
       <c r="B67" s="39">
         <v>65</v>
@@ -56764,7 +56769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="12">
+    <row r="68" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="38"/>
       <c r="B68" s="39">
         <v>66</v>
@@ -56791,7 +56796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="12">
+    <row r="69" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="38"/>
       <c r="B69" s="39">
         <v>67</v>
@@ -56818,7 +56823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="12">
+    <row r="70" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="38"/>
       <c r="B70" s="39">
         <v>68</v>
@@ -56845,7 +56850,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="12">
+    <row r="71" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="38"/>
       <c r="B71" s="39">
         <v>69</v>
@@ -56872,7 +56877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="12">
+    <row r="72" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="38"/>
       <c r="B72" s="39">
         <v>70</v>
@@ -56899,7 +56904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="12">
+    <row r="73" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="38"/>
       <c r="B73" s="39">
         <v>71</v>
@@ -56926,7 +56931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="12">
+    <row r="74" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="38"/>
       <c r="B74" s="39">
         <v>72</v>
@@ -56953,7 +56958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="12">
+    <row r="75" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="38"/>
       <c r="B75" s="39">
         <v>73</v>
@@ -56980,7 +56985,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="12">
+    <row r="76" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="38"/>
       <c r="B76" s="39">
         <v>74</v>
@@ -57007,7 +57012,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="12">
+    <row r="77" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="38"/>
       <c r="B77" s="39">
         <v>75</v>
@@ -57034,7 +57039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="12">
+    <row r="78" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="38"/>
       <c r="B78" s="39">
         <v>76</v>
@@ -57061,7 +57066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="12">
+    <row r="79" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="38"/>
       <c r="B79" s="39">
         <v>77</v>
@@ -57088,7 +57093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="12">
+    <row r="80" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="38"/>
       <c r="B80" s="39">
         <v>78</v>
@@ -57115,7 +57120,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="12">
+    <row r="81" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="38"/>
       <c r="B81" s="39">
         <v>79</v>
@@ -57142,7 +57147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="12">
+    <row r="82" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="38"/>
       <c r="B82" s="39">
         <v>80</v>
@@ -57169,7 +57174,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="12">
+    <row r="83" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="38"/>
       <c r="B83" s="39">
         <v>81</v>
@@ -57196,7 +57201,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="12">
+    <row r="84" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="38"/>
       <c r="B84" s="39">
         <v>82</v>
@@ -57223,7 +57228,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="12">
+    <row r="85" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="38"/>
       <c r="B85" s="39">
         <v>83</v>
@@ -57250,7 +57255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="12">
+    <row r="86" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="38"/>
       <c r="B86" s="39">
         <v>84</v>
@@ -57277,7 +57282,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="12">
+    <row r="87" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="38"/>
       <c r="B87" s="39">
         <v>85</v>
@@ -57304,7 +57309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="12">
+    <row r="88" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="38"/>
       <c r="B88" s="39">
         <v>86</v>
@@ -57331,7 +57336,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="12">
+    <row r="89" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="38"/>
       <c r="B89" s="39">
         <v>87</v>
@@ -57358,7 +57363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="12">
+    <row r="90" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="38"/>
       <c r="B90" s="39">
         <v>88</v>
@@ -57385,7 +57390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="12">
+    <row r="91" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="38"/>
       <c r="B91" s="39">
         <v>89</v>
@@ -57412,7 +57417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="12">
+    <row r="92" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="38"/>
       <c r="B92" s="39">
         <v>90</v>
@@ -57439,7 +57444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="12">
+    <row r="93" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="38"/>
       <c r="B93" s="39">
         <v>91</v>
@@ -57466,7 +57471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="12">
+    <row r="94" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="38"/>
       <c r="B94" s="39">
         <v>92</v>
@@ -57493,7 +57498,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="12">
+    <row r="95" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="38"/>
       <c r="B95" s="39">
         <v>93</v>
@@ -57520,7 +57525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="12">
+    <row r="96" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="38"/>
       <c r="B96" s="39">
         <v>94</v>
@@ -57547,7 +57552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="12">
+    <row r="97" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="38"/>
       <c r="B97" s="39">
         <v>95</v>
@@ -57574,7 +57579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="12">
+    <row r="98" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="38"/>
       <c r="B98" s="39">
         <v>96</v>
@@ -57604,10 +57609,5 @@
   </sheetData>
   <sheetProtection password="B946" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>